<commit_message>
updated the test script
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8F9B2FE0-2309-4663-8825-56E78E0590B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="23010" windowHeight="12960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ambassador" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:R12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>obayemi.oje@gmail.com</t>
   </si>
@@ -27,16 +29,13 @@
     <t>obayemmy92@gmail.com</t>
   </si>
   <si>
-    <t>Democracy92@</t>
-  </si>
-  <si>
     <t>ghensky.oje@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,6 +88,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -136,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -169,9 +171,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,6 +223,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,20 +415,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,17 +436,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -418,31 +454,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>